<commit_message>
Zmniejszanie i zwiększanie ilości produktów
  z 0 na 1 - dodaje produkt do listy zakupowej, z 1 na 0 - zdejmuje.
</commit_message>
<xml_diff>
--- a/Lidl.xlsx
+++ b/Lidl.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="150" windowWidth="21480" windowHeight="9795" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="150" windowWidth="21480" windowHeight="9795" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
     <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
-    <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
+    <sheet name="Lidl" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="284">
   <si>
     <t>2019—11—07</t>
   </si>
@@ -508,6 +508,366 @@
   </si>
   <si>
     <t>Razem 315,67</t>
+  </si>
+  <si>
+    <t>['</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>,' ','</t>
+  </si>
+  <si>
+    <t>],</t>
+  </si>
+  <si>
+    <t>Kasi'</t>
+  </si>
+  <si>
+    <t>Alm. Alent. Wino '</t>
+  </si>
+  <si>
+    <t>Almette Serek '</t>
+  </si>
+  <si>
+    <t>Bagietka św.czosnk '</t>
+  </si>
+  <si>
+    <t>Banany Premium św. '</t>
+  </si>
+  <si>
+    <t>Baton zboż.Chocapic '</t>
+  </si>
+  <si>
+    <t>Bella podpaski B.G.N '</t>
+  </si>
+  <si>
+    <t>BIO Ciastka owsiane '</t>
+  </si>
+  <si>
+    <t>Bułka K. św. '</t>
+  </si>
+  <si>
+    <t>C.Minis Baton zboż.'</t>
+  </si>
+  <si>
+    <t>Camembert 129g '</t>
+  </si>
+  <si>
+    <t>Chipsy Cheetos '</t>
+  </si>
+  <si>
+    <t>Chipsy Monst.Munch. '</t>
+  </si>
+  <si>
+    <t>Chipsy ziem.pap.'</t>
+  </si>
+  <si>
+    <t>Chleb raz.na ma.św.'</t>
+  </si>
+  <si>
+    <t>Chrupki BBQ'</t>
+  </si>
+  <si>
+    <t>Chust.hig.int. '</t>
+  </si>
+  <si>
+    <t>Coca—cola nap.gaz.'</t>
+  </si>
+  <si>
+    <t>Cukier wanilinowy '</t>
+  </si>
+  <si>
+    <t>Cwiartka z kurczaka '</t>
+  </si>
+  <si>
+    <t>Czek.z orz.lask. '</t>
+  </si>
+  <si>
+    <t>Czekolada z s.migdał'</t>
+  </si>
+  <si>
+    <t>Czosnek granulow.'</t>
+  </si>
+  <si>
+    <t>ćwiartka z kurczaka '</t>
+  </si>
+  <si>
+    <t>D.Szynka got.299g '</t>
+  </si>
+  <si>
+    <t>Donut Milka św '</t>
+  </si>
+  <si>
+    <t>Fasola ziel świeża '</t>
+  </si>
+  <si>
+    <t>Favita Ser '</t>
+  </si>
+  <si>
+    <t>Folia spożywcza '</t>
+  </si>
+  <si>
+    <t>Frytki mrożone 7x7 '</t>
+  </si>
+  <si>
+    <t>Granola M.Czek.—kok.'</t>
+  </si>
+  <si>
+    <t>Groszek kons.puszka'</t>
+  </si>
+  <si>
+    <t>herb.Rooibos,Pu—erh '</t>
+  </si>
+  <si>
+    <t>Herbata ziel.79g '</t>
+  </si>
+  <si>
+    <t>Herbatniki Maltanki'</t>
+  </si>
+  <si>
+    <t>Jaja L '</t>
+  </si>
+  <si>
+    <t>Jog.nat.3% b.lakt. '</t>
+  </si>
+  <si>
+    <t>Kabanosy drob.Tar. '</t>
+  </si>
+  <si>
+    <t>Kania Majonez '</t>
+  </si>
+  <si>
+    <t>Ketchup łagodny '</t>
+  </si>
+  <si>
+    <t>Kiełb. krak. sucha '</t>
+  </si>
+  <si>
+    <t>Kiełki sort. '</t>
+  </si>
+  <si>
+    <t>Kinder Bueno baton '</t>
+  </si>
+  <si>
+    <t>Koncentrat pom. '</t>
+  </si>
+  <si>
+    <t>Koperek św. '</t>
+  </si>
+  <si>
+    <t>Kopytka '</t>
+  </si>
+  <si>
+    <t>Kor. śledziowe '</t>
+  </si>
+  <si>
+    <t>Kukurydza konserw.'</t>
+  </si>
+  <si>
+    <t>Lech Fr. Lim.Mięta '</t>
+  </si>
+  <si>
+    <t>Lipton Herb.mroż. '</t>
+  </si>
+  <si>
+    <t>Lipton Ice Tea '</t>
+  </si>
+  <si>
+    <t>Liście laurowe '</t>
+  </si>
+  <si>
+    <t>Lody jogurt. 469ml '</t>
+  </si>
+  <si>
+    <t>Lody Sandwich '</t>
+  </si>
+  <si>
+    <t>Lody Twister '</t>
+  </si>
+  <si>
+    <t>Łosoś dziki 9,378 '</t>
+  </si>
+  <si>
+    <t>Łosoś wędzony199g 2'</t>
+  </si>
+  <si>
+    <t>Makaron kokard.500g '</t>
+  </si>
+  <si>
+    <t>Maseczki 2x6ml'</t>
+  </si>
+  <si>
+    <t>Masz.d.gol. Venus '</t>
+  </si>
+  <si>
+    <t>Mąka tortowa459 1kg '</t>
+  </si>
+  <si>
+    <t>Miesz chińska mroż. '</t>
+  </si>
+  <si>
+    <t>Miesz. żur. i nerk. '</t>
+  </si>
+  <si>
+    <t>Mieszanka sałat '</t>
+  </si>
+  <si>
+    <t>Mięso miel.w.—woł. '</t>
+  </si>
+  <si>
+    <t>Mięso mielone woł.Pr '</t>
+  </si>
+  <si>
+    <t>Migdały łuskane '</t>
+  </si>
+  <si>
+    <t>Mleczko wan.w czekol'</t>
+  </si>
+  <si>
+    <t>Mleko bez laktozy '</t>
+  </si>
+  <si>
+    <t>Nat.pietruszki św. '</t>
+  </si>
+  <si>
+    <t>Nekt.pomar.59%1,5L '</t>
+  </si>
+  <si>
+    <t>Nutella kr.cz.359g '</t>
+  </si>
+  <si>
+    <t>Oetker Budyń '</t>
+  </si>
+  <si>
+    <t>Ogórki ziel świeże '</t>
+  </si>
+  <si>
+    <t>Orzechy nerkow.XXL'</t>
+  </si>
+  <si>
+    <t>Paluszki serowe'</t>
+  </si>
+  <si>
+    <t>Paluszki słone '</t>
+  </si>
+  <si>
+    <t>Papr żółta św. luz'</t>
+  </si>
+  <si>
+    <t>Papryka c. świeża'</t>
+  </si>
+  <si>
+    <t>Parówki Berlinki '</t>
+  </si>
+  <si>
+    <t>Patyczki kosmetyczne '</t>
+  </si>
+  <si>
+    <t>Pieczarki świeże '</t>
+  </si>
+  <si>
+    <t>Pierogi z kap./grzyb '</t>
+  </si>
+  <si>
+    <t>Piwo Perlenb. 0,5L'</t>
+  </si>
+  <si>
+    <t>Pizza Margherit399g '</t>
+  </si>
+  <si>
+    <t>Płatki Corn Flakes '</t>
+  </si>
+  <si>
+    <t>Płatki kosmetyczne '</t>
+  </si>
+  <si>
+    <t>Pomidor kiśc świeży'</t>
+  </si>
+  <si>
+    <t>pomidory w puszce '</t>
+  </si>
+  <si>
+    <t>Popcorn do mik.sol. '</t>
+  </si>
+  <si>
+    <t>Przyprawa Majeranek '</t>
+  </si>
+  <si>
+    <t>Pstr.łososiow.wędz. '</t>
+  </si>
+  <si>
+    <t>Ptasie mleczko '</t>
+  </si>
+  <si>
+    <t>Pure Frankfurterki '</t>
+  </si>
+  <si>
+    <t>Ryż Basmati '</t>
+  </si>
+  <si>
+    <t>Schab wieprzowy b/k '</t>
+  </si>
+  <si>
+    <t>Ser Gouda '</t>
+  </si>
+  <si>
+    <t>Ser Mozzarella '</t>
+  </si>
+  <si>
+    <t>Ser topiony pl.200g '</t>
+  </si>
+  <si>
+    <t>Ser w plastrach'</t>
+  </si>
+  <si>
+    <t>Serek wiej.bez lak.'</t>
+  </si>
+  <si>
+    <t>Skrzydła z kurczaka '</t>
+  </si>
+  <si>
+    <t>Sokołów Kabanosy '</t>
+  </si>
+  <si>
+    <t>Szczypiorek św. '</t>
+  </si>
+  <si>
+    <t>Szynka got.delik.'</t>
+  </si>
+  <si>
+    <t>Szynka Szwar.kroj. '</t>
+  </si>
+  <si>
+    <t>Twaróg półtł. klin. '</t>
+  </si>
+  <si>
+    <t>Tymb.Nekt.eop29% '</t>
+  </si>
+  <si>
+    <t>Wafle ryżowe'</t>
+  </si>
+  <si>
+    <t>Wino Cardal '</t>
+  </si>
+  <si>
+    <t>Wkładki hig.long '</t>
+  </si>
+  <si>
+    <t>Worki na śmieci 69L '</t>
+  </si>
+  <si>
+    <t>Wrigley's Guma II '</t>
+  </si>
+  <si>
+    <t>Ziemniaki 5kg, św '</t>
+  </si>
+  <si>
+    <t>Zupa błyskaw. '</t>
+  </si>
+  <si>
+    <t>Żurawina susz.'</t>
   </si>
 </sst>
 </file>
@@ -1506,10 +1866,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:G164"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E62"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1519,9 +1879,10 @@
     <col min="3" max="3" width="41.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.125" customWidth="1"/>
     <col min="5" max="5" width="39.125" customWidth="1"/>
+    <col min="7" max="7" width="39.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:7" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1531,8 +1892,11 @@
       <c r="E1" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75">
+      <c r="G1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75">
       <c r="A2" s="1" t="s">
         <v>38</v>
       </c>
@@ -1542,8 +1906,11 @@
       <c r="E2" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75">
+      <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1553,8 +1920,11 @@
       <c r="E3" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75">
+      <c r="G3" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -1564,8 +1934,11 @@
       <c r="E4" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75">
+      <c r="G4" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75">
       <c r="A5" s="1" t="s">
         <v>43</v>
       </c>
@@ -1575,8 +1948,11 @@
       <c r="E5" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75">
+      <c r="G5" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75">
       <c r="A6" s="1" t="s">
         <v>39</v>
       </c>
@@ -1586,8 +1962,11 @@
       <c r="E6" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75">
+      <c r="G6" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -1597,8 +1976,11 @@
       <c r="E7" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75">
+      <c r="G7" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -1608,8 +1990,11 @@
       <c r="E8" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75">
+      <c r="G8" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -1619,8 +2004,11 @@
       <c r="E9" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75">
+      <c r="G9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -1630,8 +2018,11 @@
       <c r="E10" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75">
+      <c r="G10" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1641,8 +2032,11 @@
       <c r="E11" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75">
+      <c r="G11" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1652,8 +2046,11 @@
       <c r="E12" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75">
+      <c r="G12" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1663,8 +2060,11 @@
       <c r="E13" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75">
+      <c r="G13" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -1674,8 +2074,11 @@
       <c r="E14" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75">
+      <c r="G14" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -1685,8 +2088,11 @@
       <c r="E15" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75">
+      <c r="G15" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75">
       <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
@@ -1696,8 +2102,11 @@
       <c r="E16" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75">
+      <c r="G16" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1707,8 +2116,11 @@
       <c r="E17" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75">
+      <c r="G17" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75">
       <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
@@ -1718,8 +2130,11 @@
       <c r="E18" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75">
+      <c r="G18" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1729,8 +2144,11 @@
       <c r="E19" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75">
+      <c r="G19" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
@@ -1740,8 +2158,11 @@
       <c r="E20" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75">
+      <c r="G20" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
@@ -1751,8 +2172,11 @@
       <c r="E21" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75">
+      <c r="G21" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75">
       <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
@@ -1762,8 +2186,11 @@
       <c r="E22" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75">
+      <c r="G22" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -1773,8 +2200,11 @@
       <c r="E23" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75">
+      <c r="G23" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
@@ -1784,8 +2214,11 @@
       <c r="E24" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75">
+      <c r="G24" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75">
       <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
@@ -1795,8 +2228,11 @@
       <c r="E25" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75">
+      <c r="G25" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -1806,8 +2242,11 @@
       <c r="E26" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75">
+      <c r="G26" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
@@ -1817,8 +2256,11 @@
       <c r="E27" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75">
+      <c r="G27" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -1828,8 +2270,11 @@
       <c r="E28" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75">
+      <c r="G28" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75">
       <c r="A29" s="1" t="s">
         <v>20</v>
       </c>
@@ -1839,8 +2284,11 @@
       <c r="E29" s="1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75">
+      <c r="G29" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -1850,8 +2298,11 @@
       <c r="E30" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75">
+      <c r="G30" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75">
       <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
@@ -1861,8 +2312,11 @@
       <c r="E31" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.75">
+      <c r="G31" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
@@ -1872,8 +2326,11 @@
       <c r="E32" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="15.75">
+      <c r="G32" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15.75">
       <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
@@ -1883,8 +2340,11 @@
       <c r="E33" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="15.75">
+      <c r="G33" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15.75">
       <c r="A34" s="1" t="s">
         <v>28</v>
       </c>
@@ -1894,8 +2354,11 @@
       <c r="E34" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="15.75">
+      <c r="G34" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15.75">
       <c r="A35" s="1" t="s">
         <v>15</v>
       </c>
@@ -1905,8 +2368,11 @@
       <c r="E35" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="15.75">
+      <c r="G35" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15.75">
       <c r="A36" s="1" t="s">
         <v>1</v>
       </c>
@@ -1916,8 +2382,11 @@
       <c r="E36" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="15.75">
+      <c r="G36" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15.75">
       <c r="A37" s="1" t="s">
         <v>3</v>
       </c>
@@ -1927,8 +2396,11 @@
       <c r="E37" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="15.75">
+      <c r="G37" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15.75">
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
@@ -1938,8 +2410,11 @@
       <c r="E38" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="15.75">
+      <c r="G38" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15.75">
       <c r="A39" s="1" t="s">
         <v>7</v>
       </c>
@@ -1949,8 +2424,11 @@
       <c r="E39" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="15.75">
+      <c r="G39" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15.75">
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
@@ -1960,8 +2438,11 @@
       <c r="E40" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="15.75">
+      <c r="G40" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15.75">
       <c r="A41" s="1" t="s">
         <v>23</v>
       </c>
@@ -1971,8 +2452,11 @@
       <c r="E41" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="15.75">
+      <c r="G41" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15.75">
       <c r="A42" s="1" t="s">
         <v>13</v>
       </c>
@@ -1982,8 +2466,11 @@
       <c r="E42" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="15.75">
+      <c r="G42" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15.75">
       <c r="A43" s="1" t="s">
         <v>4</v>
       </c>
@@ -1993,8 +2480,11 @@
       <c r="E43" s="1" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="15.75">
+      <c r="G43" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15.75">
       <c r="A44" s="1" t="s">
         <v>18</v>
       </c>
@@ -2004,8 +2494,11 @@
       <c r="E44" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" ht="15.75">
+      <c r="G44" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15.75">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
@@ -2015,147 +2508,611 @@
       <c r="E45" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="15.75">
+      <c r="G45" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15.75">
       <c r="C46" s="1" t="s">
         <v>64</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="15.75">
+      <c r="G46" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="15.75">
       <c r="C47" s="1" t="s">
         <v>69</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" ht="15.75">
+      <c r="G47" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15.75">
       <c r="C48" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="49" spans="3:5" ht="15.75">
+      <c r="G48" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7" ht="15.75">
       <c r="C49" s="1" t="s">
         <v>72</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="50" spans="3:5" ht="15.75">
+      <c r="G49" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7" ht="15.75">
       <c r="C50" s="1" t="s">
         <v>88</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="51" spans="3:5" ht="15.75">
+      <c r="G50" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="3:7" ht="15.75">
       <c r="C51" s="1" t="s">
         <v>83</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="52" spans="3:5" ht="15.75">
+      <c r="G51" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="3:7" ht="15.75">
       <c r="C52" s="1" t="s">
         <v>97</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="53" spans="3:5" ht="15.75">
+      <c r="G52" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="53" spans="3:7" ht="15.75">
       <c r="C53" s="1" t="s">
         <v>103</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="54" spans="3:5" ht="15.75">
+      <c r="G53" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="54" spans="3:7" ht="15.75">
       <c r="C54" s="1" t="s">
         <v>62</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="55" spans="3:5" ht="15.75">
+      <c r="G54" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="55" spans="3:7" ht="15.75">
       <c r="C55" s="1" t="s">
         <v>86</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="56" spans="3:5" ht="15.75">
+      <c r="G55" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="56" spans="3:7" ht="15.75">
       <c r="C56" s="1" t="s">
         <v>92</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="57" spans="3:5" ht="15.75">
+      <c r="G56" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" spans="3:7" ht="15.75">
       <c r="C57" s="1" t="s">
         <v>89</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="58" spans="3:5" ht="15.75">
+      <c r="G57" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="3:7" ht="15.75">
       <c r="C58" s="1" t="s">
         <v>105</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="59" spans="3:5" ht="15.75">
+      <c r="G58" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="3:7" ht="15.75">
       <c r="C59" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="60" spans="3:5" ht="15.75">
+      <c r="G59" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="3:7" ht="15.75">
       <c r="C60" s="1" t="s">
         <v>59</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="61" spans="3:5" ht="15.75">
+      <c r="G60" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="61" spans="3:7" ht="15.75">
       <c r="C61" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="62" spans="3:5" ht="15.75">
+      <c r="G61" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="62" spans="3:7" ht="15.75">
       <c r="C62" s="1" t="s">
         <v>106</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="63" spans="3:5" ht="15.75">
+      <c r="G62" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="63" spans="3:7" ht="15.75">
       <c r="E63" s="1" t="s">
         <v>163</v>
       </c>
+      <c r="G63" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64" spans="3:7" ht="15.75">
+      <c r="G64" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="7:7" ht="15.75">
+      <c r="G65" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="66" spans="7:7" ht="15.75">
+      <c r="G66" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="67" spans="7:7" ht="15.75">
+      <c r="G67" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" spans="7:7" ht="15.75">
+      <c r="G68" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="69" spans="7:7" ht="15.75">
+      <c r="G69" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="70" spans="7:7" ht="15.75">
+      <c r="G70" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="71" spans="7:7" ht="15.75">
+      <c r="G71" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="72" spans="7:7" ht="15.75">
+      <c r="G72" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="73" spans="7:7" ht="15.75">
+      <c r="G73" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="74" spans="7:7" ht="15.75">
+      <c r="G74" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="75" spans="7:7" ht="15.75">
+      <c r="G75" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="76" spans="7:7" ht="15.75">
+      <c r="G76" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="77" spans="7:7" ht="15.75">
+      <c r="G77" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="78" spans="7:7" ht="15.75">
+      <c r="G78" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="79" spans="7:7" ht="15.75">
+      <c r="G79" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="80" spans="7:7" ht="15.75">
+      <c r="G80" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="81" spans="7:7" ht="15.75">
+      <c r="G81" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="82" spans="7:7" ht="15.75">
+      <c r="G82" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="83" spans="7:7" ht="15.75">
+      <c r="G83" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="7:7" ht="15.75">
+      <c r="G84" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="85" spans="7:7" ht="15.75">
+      <c r="G85" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="86" spans="7:7" ht="15.75">
+      <c r="G86" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="87" spans="7:7" ht="15.75">
+      <c r="G87" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="88" spans="7:7" ht="15.75">
+      <c r="G88" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="89" spans="7:7" ht="15.75">
+      <c r="G89" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="90" spans="7:7" ht="15.75">
+      <c r="G90" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="91" spans="7:7" ht="15.75">
+      <c r="G91" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="92" spans="7:7" ht="15.75">
+      <c r="G92" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="93" spans="7:7" ht="15.75">
+      <c r="G93" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="94" spans="7:7" ht="15.75">
+      <c r="G94" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="95" spans="7:7" ht="15.75">
+      <c r="G95" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="96" spans="7:7" ht="15.75">
+      <c r="G96" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="97" spans="7:7" ht="15.75">
+      <c r="G97" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="98" spans="7:7" ht="15.75">
+      <c r="G98" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="99" spans="7:7" ht="15.75">
+      <c r="G99" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="100" spans="7:7" ht="15.75">
+      <c r="G100" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="101" spans="7:7" ht="15.75">
+      <c r="G101" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="102" spans="7:7" ht="15.75">
+      <c r="G102" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="103" spans="7:7" ht="15.75">
+      <c r="G103" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="104" spans="7:7" ht="15.75">
+      <c r="G104" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="105" spans="7:7" ht="15.75">
+      <c r="G105" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="106" spans="7:7" ht="15.75">
+      <c r="G106" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="107" spans="7:7" ht="15.75">
+      <c r="G107" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="108" spans="7:7" ht="15.75">
+      <c r="G108" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" spans="7:7" ht="15.75">
+      <c r="G109" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="110" spans="7:7" ht="15.75">
+      <c r="G110" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="111" spans="7:7" ht="15.75">
+      <c r="G111" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="112" spans="7:7" ht="15.75">
+      <c r="G112" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="113" spans="7:7" ht="15.75">
+      <c r="G113" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="114" spans="7:7" ht="15.75">
+      <c r="G114" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="115" spans="7:7" ht="15.75">
+      <c r="G115" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="116" spans="7:7" ht="15.75">
+      <c r="G116" s="1"/>
+    </row>
+    <row r="117" spans="7:7" ht="15.75">
+      <c r="G117" s="1"/>
+    </row>
+    <row r="118" spans="7:7" ht="15.75">
+      <c r="G118" s="1"/>
+    </row>
+    <row r="119" spans="7:7" ht="15.75">
+      <c r="G119" s="1"/>
+    </row>
+    <row r="120" spans="7:7" ht="15.75">
+      <c r="G120" s="1"/>
+    </row>
+    <row r="121" spans="7:7" ht="15.75">
+      <c r="G121" s="1"/>
+    </row>
+    <row r="122" spans="7:7" ht="15.75">
+      <c r="G122" s="1"/>
+    </row>
+    <row r="123" spans="7:7" ht="15.75">
+      <c r="G123" s="1"/>
+    </row>
+    <row r="124" spans="7:7" ht="15.75">
+      <c r="G124" s="1"/>
+    </row>
+    <row r="125" spans="7:7" ht="15.75">
+      <c r="G125" s="1"/>
+    </row>
+    <row r="126" spans="7:7" ht="15.75">
+      <c r="G126" s="1"/>
+    </row>
+    <row r="127" spans="7:7" ht="15.75">
+      <c r="G127" s="1"/>
+    </row>
+    <row r="128" spans="7:7" ht="15.75">
+      <c r="G128" s="1"/>
+    </row>
+    <row r="129" spans="7:7" ht="15.75">
+      <c r="G129" s="1"/>
+    </row>
+    <row r="130" spans="7:7" ht="15.75">
+      <c r="G130" s="1"/>
+    </row>
+    <row r="131" spans="7:7" ht="15.75">
+      <c r="G131" s="1"/>
+    </row>
+    <row r="132" spans="7:7" ht="15.75">
+      <c r="G132" s="1"/>
+    </row>
+    <row r="133" spans="7:7" ht="15.75">
+      <c r="G133" s="1"/>
+    </row>
+    <row r="134" spans="7:7" ht="15.75">
+      <c r="G134" s="1"/>
+    </row>
+    <row r="135" spans="7:7" ht="15.75">
+      <c r="G135" s="1"/>
+    </row>
+    <row r="136" spans="7:7" ht="15.75">
+      <c r="G136" s="1"/>
+    </row>
+    <row r="137" spans="7:7" ht="15.75">
+      <c r="G137" s="1"/>
+    </row>
+    <row r="138" spans="7:7" ht="15.75">
+      <c r="G138" s="1"/>
+    </row>
+    <row r="139" spans="7:7" ht="15.75">
+      <c r="G139" s="1"/>
+    </row>
+    <row r="140" spans="7:7" ht="15.75">
+      <c r="G140" s="1"/>
+    </row>
+    <row r="141" spans="7:7" ht="15.75">
+      <c r="G141" s="1"/>
+    </row>
+    <row r="142" spans="7:7" ht="15.75">
+      <c r="G142" s="1"/>
+    </row>
+    <row r="143" spans="7:7" ht="15.75">
+      <c r="G143" s="1"/>
+    </row>
+    <row r="144" spans="7:7" ht="15.75">
+      <c r="G144" s="1"/>
+    </row>
+    <row r="145" spans="7:7" ht="15.75">
+      <c r="G145" s="1"/>
+    </row>
+    <row r="146" spans="7:7" ht="15.75">
+      <c r="G146" s="1"/>
+    </row>
+    <row r="147" spans="7:7" ht="15.75">
+      <c r="G147" s="1"/>
+    </row>
+    <row r="148" spans="7:7" ht="15.75">
+      <c r="G148" s="1"/>
+    </row>
+    <row r="149" spans="7:7" ht="15.75">
+      <c r="G149" s="1"/>
+    </row>
+    <row r="150" spans="7:7" ht="15.75">
+      <c r="G150" s="1"/>
+    </row>
+    <row r="151" spans="7:7" ht="15.75">
+      <c r="G151" s="1"/>
+    </row>
+    <row r="152" spans="7:7" ht="15.75">
+      <c r="G152" s="1"/>
+    </row>
+    <row r="153" spans="7:7" ht="15.75">
+      <c r="G153" s="1"/>
+    </row>
+    <row r="154" spans="7:7" ht="15.75">
+      <c r="G154" s="1"/>
+    </row>
+    <row r="155" spans="7:7" ht="15.75">
+      <c r="G155" s="1"/>
+    </row>
+    <row r="156" spans="7:7" ht="15.75">
+      <c r="G156" s="1"/>
+    </row>
+    <row r="157" spans="7:7" ht="15.75">
+      <c r="G157" s="1"/>
+    </row>
+    <row r="158" spans="7:7" ht="15.75">
+      <c r="G158" s="1"/>
+    </row>
+    <row r="159" spans="7:7" ht="15.75">
+      <c r="G159" s="1"/>
+    </row>
+    <row r="160" spans="7:7" ht="15.75">
+      <c r="G160" s="1"/>
+    </row>
+    <row r="161" spans="7:7" ht="15.75">
+      <c r="G161" s="1"/>
+    </row>
+    <row r="162" spans="7:7" ht="15.75">
+      <c r="G162" s="1"/>
+    </row>
+    <row r="163" spans="7:7" ht="15.75">
+      <c r="G163" s="1"/>
+    </row>
+    <row r="164" spans="7:7" ht="15.75">
+      <c r="G164" s="1"/>
     </row>
   </sheetData>
   <sortState ref="E2:E62">
@@ -2167,12 +3124,2672 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="1.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F3" t="s">
+        <v>168</v>
+      </c>
+      <c r="G3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F4" t="s">
+        <v>168</v>
+      </c>
+      <c r="G4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" t="s">
+        <v>279</v>
+      </c>
+      <c r="C5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F5" t="s">
+        <v>168</v>
+      </c>
+      <c r="G5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>166</v>
+      </c>
+      <c r="F6" t="s">
+        <v>168</v>
+      </c>
+      <c r="G6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" t="s">
+        <v>277</v>
+      </c>
+      <c r="C7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F7" t="s">
+        <v>168</v>
+      </c>
+      <c r="G7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B8" t="s">
+        <v>276</v>
+      </c>
+      <c r="C8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>166</v>
+      </c>
+      <c r="F8" t="s">
+        <v>168</v>
+      </c>
+      <c r="G8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9" t="s">
+        <v>275</v>
+      </c>
+      <c r="C9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>166</v>
+      </c>
+      <c r="F9" t="s">
+        <v>168</v>
+      </c>
+      <c r="G9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>164</v>
+      </c>
+      <c r="B10" t="s">
+        <v>274</v>
+      </c>
+      <c r="C10" t="s">
+        <v>165</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F10" t="s">
+        <v>168</v>
+      </c>
+      <c r="G10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B11" t="s">
+        <v>273</v>
+      </c>
+      <c r="C11" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>166</v>
+      </c>
+      <c r="F11" t="s">
+        <v>168</v>
+      </c>
+      <c r="G11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>164</v>
+      </c>
+      <c r="B12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C12" t="s">
+        <v>165</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>166</v>
+      </c>
+      <c r="F12" t="s">
+        <v>168</v>
+      </c>
+      <c r="G12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>164</v>
+      </c>
+      <c r="B13" t="s">
+        <v>271</v>
+      </c>
+      <c r="C13" t="s">
+        <v>165</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>166</v>
+      </c>
+      <c r="F13" t="s">
+        <v>168</v>
+      </c>
+      <c r="G13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>164</v>
+      </c>
+      <c r="B14" t="s">
+        <v>270</v>
+      </c>
+      <c r="C14" t="s">
+        <v>165</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>166</v>
+      </c>
+      <c r="F14" t="s">
+        <v>168</v>
+      </c>
+      <c r="G14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>164</v>
+      </c>
+      <c r="B15" t="s">
+        <v>269</v>
+      </c>
+      <c r="C15" t="s">
+        <v>165</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>166</v>
+      </c>
+      <c r="F15" t="s">
+        <v>168</v>
+      </c>
+      <c r="G15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B16" t="s">
+        <v>268</v>
+      </c>
+      <c r="C16" t="s">
+        <v>165</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>166</v>
+      </c>
+      <c r="F16" t="s">
+        <v>168</v>
+      </c>
+      <c r="G16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>164</v>
+      </c>
+      <c r="B17" t="s">
+        <v>267</v>
+      </c>
+      <c r="C17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>166</v>
+      </c>
+      <c r="F17" t="s">
+        <v>168</v>
+      </c>
+      <c r="G17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>164</v>
+      </c>
+      <c r="B18" t="s">
+        <v>266</v>
+      </c>
+      <c r="C18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>166</v>
+      </c>
+      <c r="F18" t="s">
+        <v>168</v>
+      </c>
+      <c r="G18" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>164</v>
+      </c>
+      <c r="B19" t="s">
+        <v>265</v>
+      </c>
+      <c r="C19" t="s">
+        <v>165</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>166</v>
+      </c>
+      <c r="F19" t="s">
+        <v>168</v>
+      </c>
+      <c r="G19" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>164</v>
+      </c>
+      <c r="B20" t="s">
+        <v>264</v>
+      </c>
+      <c r="C20" t="s">
+        <v>165</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>166</v>
+      </c>
+      <c r="F20" t="s">
+        <v>168</v>
+      </c>
+      <c r="G20" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>164</v>
+      </c>
+      <c r="B21" t="s">
+        <v>263</v>
+      </c>
+      <c r="C21" t="s">
+        <v>165</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>166</v>
+      </c>
+      <c r="F21" t="s">
+        <v>168</v>
+      </c>
+      <c r="G21" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>164</v>
+      </c>
+      <c r="B22" t="s">
+        <v>262</v>
+      </c>
+      <c r="C22" t="s">
+        <v>165</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>166</v>
+      </c>
+      <c r="F22" t="s">
+        <v>168</v>
+      </c>
+      <c r="G22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>164</v>
+      </c>
+      <c r="B23" t="s">
+        <v>261</v>
+      </c>
+      <c r="C23" t="s">
+        <v>165</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>166</v>
+      </c>
+      <c r="F23" t="s">
+        <v>168</v>
+      </c>
+      <c r="G23" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>164</v>
+      </c>
+      <c r="B24" t="s">
+        <v>260</v>
+      </c>
+      <c r="C24" t="s">
+        <v>165</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>166</v>
+      </c>
+      <c r="F24" t="s">
+        <v>168</v>
+      </c>
+      <c r="G24" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>164</v>
+      </c>
+      <c r="B25" t="s">
+        <v>259</v>
+      </c>
+      <c r="C25" t="s">
+        <v>165</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>166</v>
+      </c>
+      <c r="F25" t="s">
+        <v>168</v>
+      </c>
+      <c r="G25" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>164</v>
+      </c>
+      <c r="B26" t="s">
+        <v>258</v>
+      </c>
+      <c r="C26" t="s">
+        <v>165</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>166</v>
+      </c>
+      <c r="F26" t="s">
+        <v>168</v>
+      </c>
+      <c r="G26" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>164</v>
+      </c>
+      <c r="B27" t="s">
+        <v>257</v>
+      </c>
+      <c r="C27" t="s">
+        <v>165</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>166</v>
+      </c>
+      <c r="F27" t="s">
+        <v>168</v>
+      </c>
+      <c r="G27" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>164</v>
+      </c>
+      <c r="B28" t="s">
+        <v>256</v>
+      </c>
+      <c r="C28" t="s">
+        <v>165</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>166</v>
+      </c>
+      <c r="F28" t="s">
+        <v>168</v>
+      </c>
+      <c r="G28" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>164</v>
+      </c>
+      <c r="B29" t="s">
+        <v>255</v>
+      </c>
+      <c r="C29" t="s">
+        <v>165</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>166</v>
+      </c>
+      <c r="F29" t="s">
+        <v>168</v>
+      </c>
+      <c r="G29" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>164</v>
+      </c>
+      <c r="B30" t="s">
+        <v>254</v>
+      </c>
+      <c r="C30" t="s">
+        <v>165</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>166</v>
+      </c>
+      <c r="F30" t="s">
+        <v>168</v>
+      </c>
+      <c r="G30" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>164</v>
+      </c>
+      <c r="B31" t="s">
+        <v>253</v>
+      </c>
+      <c r="C31" t="s">
+        <v>165</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>166</v>
+      </c>
+      <c r="F31" t="s">
+        <v>168</v>
+      </c>
+      <c r="G31" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>164</v>
+      </c>
+      <c r="B32" t="s">
+        <v>252</v>
+      </c>
+      <c r="C32" t="s">
+        <v>165</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>166</v>
+      </c>
+      <c r="F32" t="s">
+        <v>168</v>
+      </c>
+      <c r="G32" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>164</v>
+      </c>
+      <c r="B33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C33" t="s">
+        <v>165</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>166</v>
+      </c>
+      <c r="F33" t="s">
+        <v>168</v>
+      </c>
+      <c r="G33" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>164</v>
+      </c>
+      <c r="B34" t="s">
+        <v>250</v>
+      </c>
+      <c r="C34" t="s">
+        <v>165</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>166</v>
+      </c>
+      <c r="F34" t="s">
+        <v>168</v>
+      </c>
+      <c r="G34" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>164</v>
+      </c>
+      <c r="B35" t="s">
+        <v>249</v>
+      </c>
+      <c r="C35" t="s">
+        <v>165</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>166</v>
+      </c>
+      <c r="F35" t="s">
+        <v>168</v>
+      </c>
+      <c r="G35" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>164</v>
+      </c>
+      <c r="B36" t="s">
+        <v>248</v>
+      </c>
+      <c r="C36" t="s">
+        <v>165</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>166</v>
+      </c>
+      <c r="F36" t="s">
+        <v>168</v>
+      </c>
+      <c r="G36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>164</v>
+      </c>
+      <c r="B37" t="s">
+        <v>247</v>
+      </c>
+      <c r="C37" t="s">
+        <v>165</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>166</v>
+      </c>
+      <c r="F37" t="s">
+        <v>168</v>
+      </c>
+      <c r="G37" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>164</v>
+      </c>
+      <c r="B38" t="s">
+        <v>246</v>
+      </c>
+      <c r="C38" t="s">
+        <v>165</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>166</v>
+      </c>
+      <c r="F38" t="s">
+        <v>168</v>
+      </c>
+      <c r="G38" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>164</v>
+      </c>
+      <c r="B39" t="s">
+        <v>245</v>
+      </c>
+      <c r="C39" t="s">
+        <v>165</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>166</v>
+      </c>
+      <c r="F39" t="s">
+        <v>168</v>
+      </c>
+      <c r="G39" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>164</v>
+      </c>
+      <c r="B40" t="s">
+        <v>244</v>
+      </c>
+      <c r="C40" t="s">
+        <v>165</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>166</v>
+      </c>
+      <c r="F40" t="s">
+        <v>168</v>
+      </c>
+      <c r="G40" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>164</v>
+      </c>
+      <c r="B41" t="s">
+        <v>243</v>
+      </c>
+      <c r="C41" t="s">
+        <v>165</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>166</v>
+      </c>
+      <c r="F41" t="s">
+        <v>168</v>
+      </c>
+      <c r="G41" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
+        <v>164</v>
+      </c>
+      <c r="B42" t="s">
+        <v>242</v>
+      </c>
+      <c r="C42" t="s">
+        <v>165</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42" t="s">
+        <v>166</v>
+      </c>
+      <c r="F42" t="s">
+        <v>168</v>
+      </c>
+      <c r="G42" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>164</v>
+      </c>
+      <c r="B43" t="s">
+        <v>241</v>
+      </c>
+      <c r="C43" t="s">
+        <v>165</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>166</v>
+      </c>
+      <c r="F43" t="s">
+        <v>168</v>
+      </c>
+      <c r="G43" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>164</v>
+      </c>
+      <c r="B44" t="s">
+        <v>240</v>
+      </c>
+      <c r="C44" t="s">
+        <v>165</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44" t="s">
+        <v>166</v>
+      </c>
+      <c r="F44" t="s">
+        <v>168</v>
+      </c>
+      <c r="G44" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>164</v>
+      </c>
+      <c r="B45" t="s">
+        <v>239</v>
+      </c>
+      <c r="C45" t="s">
+        <v>165</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45" t="s">
+        <v>166</v>
+      </c>
+      <c r="F45" t="s">
+        <v>168</v>
+      </c>
+      <c r="G45" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
+        <v>164</v>
+      </c>
+      <c r="B46" t="s">
+        <v>238</v>
+      </c>
+      <c r="C46" t="s">
+        <v>165</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46" t="s">
+        <v>166</v>
+      </c>
+      <c r="F46" t="s">
+        <v>168</v>
+      </c>
+      <c r="G46" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" t="s">
+        <v>164</v>
+      </c>
+      <c r="B47" t="s">
+        <v>237</v>
+      </c>
+      <c r="C47" t="s">
+        <v>165</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47" t="s">
+        <v>166</v>
+      </c>
+      <c r="F47" t="s">
+        <v>168</v>
+      </c>
+      <c r="G47" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" t="s">
+        <v>164</v>
+      </c>
+      <c r="B48" t="s">
+        <v>236</v>
+      </c>
+      <c r="C48" t="s">
+        <v>165</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48" t="s">
+        <v>166</v>
+      </c>
+      <c r="F48" t="s">
+        <v>168</v>
+      </c>
+      <c r="G48" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
+        <v>164</v>
+      </c>
+      <c r="B49" t="s">
+        <v>235</v>
+      </c>
+      <c r="C49" t="s">
+        <v>165</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49" t="s">
+        <v>166</v>
+      </c>
+      <c r="F49" t="s">
+        <v>168</v>
+      </c>
+      <c r="G49" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" t="s">
+        <v>164</v>
+      </c>
+      <c r="B50" t="s">
+        <v>234</v>
+      </c>
+      <c r="C50" t="s">
+        <v>165</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50" t="s">
+        <v>166</v>
+      </c>
+      <c r="F50" t="s">
+        <v>168</v>
+      </c>
+      <c r="G50" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" t="s">
+        <v>164</v>
+      </c>
+      <c r="B51" t="s">
+        <v>233</v>
+      </c>
+      <c r="C51" t="s">
+        <v>165</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51" t="s">
+        <v>166</v>
+      </c>
+      <c r="F51" t="s">
+        <v>168</v>
+      </c>
+      <c r="G51" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" t="s">
+        <v>164</v>
+      </c>
+      <c r="B52" t="s">
+        <v>232</v>
+      </c>
+      <c r="C52" t="s">
+        <v>165</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52" t="s">
+        <v>166</v>
+      </c>
+      <c r="F52" t="s">
+        <v>168</v>
+      </c>
+      <c r="G52" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" t="s">
+        <v>164</v>
+      </c>
+      <c r="B53" t="s">
+        <v>231</v>
+      </c>
+      <c r="C53" t="s">
+        <v>165</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53" t="s">
+        <v>166</v>
+      </c>
+      <c r="F53" t="s">
+        <v>168</v>
+      </c>
+      <c r="G53" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" t="s">
+        <v>164</v>
+      </c>
+      <c r="B54" t="s">
+        <v>230</v>
+      </c>
+      <c r="C54" t="s">
+        <v>165</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54" t="s">
+        <v>166</v>
+      </c>
+      <c r="F54" t="s">
+        <v>168</v>
+      </c>
+      <c r="G54" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" t="s">
+        <v>164</v>
+      </c>
+      <c r="B55" t="s">
+        <v>229</v>
+      </c>
+      <c r="C55" t="s">
+        <v>165</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55" t="s">
+        <v>166</v>
+      </c>
+      <c r="F55" t="s">
+        <v>168</v>
+      </c>
+      <c r="G55" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" t="s">
+        <v>164</v>
+      </c>
+      <c r="B56" t="s">
+        <v>228</v>
+      </c>
+      <c r="C56" t="s">
+        <v>165</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56" t="s">
+        <v>166</v>
+      </c>
+      <c r="F56" t="s">
+        <v>168</v>
+      </c>
+      <c r="G56" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" t="s">
+        <v>164</v>
+      </c>
+      <c r="B57" t="s">
+        <v>227</v>
+      </c>
+      <c r="C57" t="s">
+        <v>165</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57" t="s">
+        <v>166</v>
+      </c>
+      <c r="F57" t="s">
+        <v>168</v>
+      </c>
+      <c r="G57" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" t="s">
+        <v>164</v>
+      </c>
+      <c r="B58" t="s">
+        <v>226</v>
+      </c>
+      <c r="C58" t="s">
+        <v>165</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58" t="s">
+        <v>166</v>
+      </c>
+      <c r="F58" t="s">
+        <v>168</v>
+      </c>
+      <c r="G58" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" t="s">
+        <v>164</v>
+      </c>
+      <c r="B59" t="s">
+        <v>225</v>
+      </c>
+      <c r="C59" t="s">
+        <v>165</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59" t="s">
+        <v>166</v>
+      </c>
+      <c r="F59" t="s">
+        <v>168</v>
+      </c>
+      <c r="G59" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" t="s">
+        <v>164</v>
+      </c>
+      <c r="B60" t="s">
+        <v>224</v>
+      </c>
+      <c r="C60" t="s">
+        <v>165</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60" t="s">
+        <v>166</v>
+      </c>
+      <c r="F60" t="s">
+        <v>168</v>
+      </c>
+      <c r="G60" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" t="s">
+        <v>164</v>
+      </c>
+      <c r="B61" t="s">
+        <v>223</v>
+      </c>
+      <c r="C61" t="s">
+        <v>165</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61" t="s">
+        <v>166</v>
+      </c>
+      <c r="F61" t="s">
+        <v>168</v>
+      </c>
+      <c r="G61" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" t="s">
+        <v>164</v>
+      </c>
+      <c r="B62" t="s">
+        <v>222</v>
+      </c>
+      <c r="C62" t="s">
+        <v>165</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62" t="s">
+        <v>166</v>
+      </c>
+      <c r="F62" t="s">
+        <v>168</v>
+      </c>
+      <c r="G62" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" t="s">
+        <v>164</v>
+      </c>
+      <c r="B63" t="s">
+        <v>221</v>
+      </c>
+      <c r="C63" t="s">
+        <v>165</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63" t="s">
+        <v>166</v>
+      </c>
+      <c r="F63" t="s">
+        <v>168</v>
+      </c>
+      <c r="G63" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" t="s">
+        <v>164</v>
+      </c>
+      <c r="B64" t="s">
+        <v>220</v>
+      </c>
+      <c r="C64" t="s">
+        <v>165</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64" t="s">
+        <v>166</v>
+      </c>
+      <c r="F64" t="s">
+        <v>168</v>
+      </c>
+      <c r="G64" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" t="s">
+        <v>164</v>
+      </c>
+      <c r="B65" t="s">
+        <v>219</v>
+      </c>
+      <c r="C65" t="s">
+        <v>165</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65" t="s">
+        <v>166</v>
+      </c>
+      <c r="F65" t="s">
+        <v>168</v>
+      </c>
+      <c r="G65" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" t="s">
+        <v>164</v>
+      </c>
+      <c r="B66" t="s">
+        <v>218</v>
+      </c>
+      <c r="C66" t="s">
+        <v>165</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66" t="s">
+        <v>166</v>
+      </c>
+      <c r="F66" t="s">
+        <v>168</v>
+      </c>
+      <c r="G66" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" t="s">
+        <v>164</v>
+      </c>
+      <c r="B67" t="s">
+        <v>217</v>
+      </c>
+      <c r="C67" t="s">
+        <v>165</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67" t="s">
+        <v>166</v>
+      </c>
+      <c r="F67" t="s">
+        <v>168</v>
+      </c>
+      <c r="G67" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" t="s">
+        <v>164</v>
+      </c>
+      <c r="B68" t="s">
+        <v>216</v>
+      </c>
+      <c r="C68" t="s">
+        <v>165</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68" t="s">
+        <v>166</v>
+      </c>
+      <c r="F68" t="s">
+        <v>168</v>
+      </c>
+      <c r="G68" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
+        <v>164</v>
+      </c>
+      <c r="B69" t="s">
+        <v>215</v>
+      </c>
+      <c r="C69" t="s">
+        <v>165</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69" t="s">
+        <v>166</v>
+      </c>
+      <c r="F69" t="s">
+        <v>168</v>
+      </c>
+      <c r="G69" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" t="s">
+        <v>164</v>
+      </c>
+      <c r="B70" t="s">
+        <v>214</v>
+      </c>
+      <c r="C70" t="s">
+        <v>165</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70" t="s">
+        <v>166</v>
+      </c>
+      <c r="F70" t="s">
+        <v>168</v>
+      </c>
+      <c r="G70" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" t="s">
+        <v>164</v>
+      </c>
+      <c r="B71" t="s">
+        <v>213</v>
+      </c>
+      <c r="C71" t="s">
+        <v>165</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71" t="s">
+        <v>166</v>
+      </c>
+      <c r="F71" t="s">
+        <v>168</v>
+      </c>
+      <c r="G71" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" t="s">
+        <v>164</v>
+      </c>
+      <c r="B72" t="s">
+        <v>212</v>
+      </c>
+      <c r="C72" t="s">
+        <v>165</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72" t="s">
+        <v>166</v>
+      </c>
+      <c r="F72" t="s">
+        <v>168</v>
+      </c>
+      <c r="G72" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" t="s">
+        <v>164</v>
+      </c>
+      <c r="B73" t="s">
+        <v>211</v>
+      </c>
+      <c r="C73" t="s">
+        <v>165</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73" t="s">
+        <v>166</v>
+      </c>
+      <c r="F73" t="s">
+        <v>168</v>
+      </c>
+      <c r="G73" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" t="s">
+        <v>164</v>
+      </c>
+      <c r="B74" t="s">
+        <v>210</v>
+      </c>
+      <c r="C74" t="s">
+        <v>165</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74" t="s">
+        <v>166</v>
+      </c>
+      <c r="F74" t="s">
+        <v>168</v>
+      </c>
+      <c r="G74" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" t="s">
+        <v>164</v>
+      </c>
+      <c r="B75" t="s">
+        <v>209</v>
+      </c>
+      <c r="C75" t="s">
+        <v>165</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75" t="s">
+        <v>166</v>
+      </c>
+      <c r="F75" t="s">
+        <v>168</v>
+      </c>
+      <c r="G75" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" t="s">
+        <v>164</v>
+      </c>
+      <c r="B76" t="s">
+        <v>208</v>
+      </c>
+      <c r="C76" t="s">
+        <v>165</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76" t="s">
+        <v>166</v>
+      </c>
+      <c r="F76" t="s">
+        <v>168</v>
+      </c>
+      <c r="G76" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" t="s">
+        <v>164</v>
+      </c>
+      <c r="B77" t="s">
+        <v>207</v>
+      </c>
+      <c r="C77" t="s">
+        <v>165</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77" t="s">
+        <v>166</v>
+      </c>
+      <c r="F77" t="s">
+        <v>168</v>
+      </c>
+      <c r="G77" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" t="s">
+        <v>164</v>
+      </c>
+      <c r="B78" t="s">
+        <v>206</v>
+      </c>
+      <c r="C78" t="s">
+        <v>165</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78" t="s">
+        <v>166</v>
+      </c>
+      <c r="F78" t="s">
+        <v>168</v>
+      </c>
+      <c r="G78" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" t="s">
+        <v>164</v>
+      </c>
+      <c r="B79" t="s">
+        <v>205</v>
+      </c>
+      <c r="C79" t="s">
+        <v>165</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79" t="s">
+        <v>166</v>
+      </c>
+      <c r="F79" t="s">
+        <v>168</v>
+      </c>
+      <c r="G79" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" t="s">
+        <v>164</v>
+      </c>
+      <c r="B80" t="s">
+        <v>204</v>
+      </c>
+      <c r="C80" t="s">
+        <v>165</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80" t="s">
+        <v>166</v>
+      </c>
+      <c r="F80" t="s">
+        <v>168</v>
+      </c>
+      <c r="G80" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" t="s">
+        <v>164</v>
+      </c>
+      <c r="B81" t="s">
+        <v>203</v>
+      </c>
+      <c r="C81" t="s">
+        <v>165</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81" t="s">
+        <v>166</v>
+      </c>
+      <c r="F81" t="s">
+        <v>168</v>
+      </c>
+      <c r="G81" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" t="s">
+        <v>164</v>
+      </c>
+      <c r="B82" t="s">
+        <v>202</v>
+      </c>
+      <c r="C82" t="s">
+        <v>165</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82" t="s">
+        <v>166</v>
+      </c>
+      <c r="F82" t="s">
+        <v>168</v>
+      </c>
+      <c r="G82" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" t="s">
+        <v>201</v>
+      </c>
+      <c r="C83" t="s">
+        <v>165</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83" t="s">
+        <v>166</v>
+      </c>
+      <c r="F83" t="s">
+        <v>168</v>
+      </c>
+      <c r="G83" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" t="s">
+        <v>164</v>
+      </c>
+      <c r="B84" t="s">
+        <v>200</v>
+      </c>
+      <c r="C84" t="s">
+        <v>165</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84" t="s">
+        <v>166</v>
+      </c>
+      <c r="F84" t="s">
+        <v>168</v>
+      </c>
+      <c r="G84" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" t="s">
+        <v>164</v>
+      </c>
+      <c r="B85" t="s">
+        <v>199</v>
+      </c>
+      <c r="C85" t="s">
+        <v>165</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85" t="s">
+        <v>166</v>
+      </c>
+      <c r="F85" t="s">
+        <v>168</v>
+      </c>
+      <c r="G85" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" t="s">
+        <v>164</v>
+      </c>
+      <c r="B86" t="s">
+        <v>198</v>
+      </c>
+      <c r="C86" t="s">
+        <v>165</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86" t="s">
+        <v>166</v>
+      </c>
+      <c r="F86" t="s">
+        <v>168</v>
+      </c>
+      <c r="G86" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" t="s">
+        <v>164</v>
+      </c>
+      <c r="B87" t="s">
+        <v>197</v>
+      </c>
+      <c r="C87" t="s">
+        <v>165</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87" t="s">
+        <v>166</v>
+      </c>
+      <c r="F87" t="s">
+        <v>168</v>
+      </c>
+      <c r="G87" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" t="s">
+        <v>164</v>
+      </c>
+      <c r="B88" t="s">
+        <v>196</v>
+      </c>
+      <c r="C88" t="s">
+        <v>165</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88" t="s">
+        <v>166</v>
+      </c>
+      <c r="F88" t="s">
+        <v>168</v>
+      </c>
+      <c r="G88" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" t="s">
+        <v>164</v>
+      </c>
+      <c r="B89" t="s">
+        <v>195</v>
+      </c>
+      <c r="C89" t="s">
+        <v>165</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89" t="s">
+        <v>166</v>
+      </c>
+      <c r="F89" t="s">
+        <v>168</v>
+      </c>
+      <c r="G89" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" t="s">
+        <v>164</v>
+      </c>
+      <c r="B90" t="s">
+        <v>194</v>
+      </c>
+      <c r="C90" t="s">
+        <v>165</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90" t="s">
+        <v>166</v>
+      </c>
+      <c r="F90" t="s">
+        <v>168</v>
+      </c>
+      <c r="G90" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" t="s">
+        <v>164</v>
+      </c>
+      <c r="B91" t="s">
+        <v>193</v>
+      </c>
+      <c r="C91" t="s">
+        <v>165</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91" t="s">
+        <v>166</v>
+      </c>
+      <c r="F91" t="s">
+        <v>168</v>
+      </c>
+      <c r="G91" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" t="s">
+        <v>164</v>
+      </c>
+      <c r="B92" t="s">
+        <v>192</v>
+      </c>
+      <c r="C92" t="s">
+        <v>165</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92" t="s">
+        <v>166</v>
+      </c>
+      <c r="F92" t="s">
+        <v>168</v>
+      </c>
+      <c r="G92" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" t="s">
+        <v>164</v>
+      </c>
+      <c r="B93" t="s">
+        <v>191</v>
+      </c>
+      <c r="C93" t="s">
+        <v>165</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93" t="s">
+        <v>166</v>
+      </c>
+      <c r="F93" t="s">
+        <v>168</v>
+      </c>
+      <c r="G93" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" t="s">
+        <v>164</v>
+      </c>
+      <c r="B94" t="s">
+        <v>190</v>
+      </c>
+      <c r="C94" t="s">
+        <v>165</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94" t="s">
+        <v>166</v>
+      </c>
+      <c r="F94" t="s">
+        <v>168</v>
+      </c>
+      <c r="G94" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95" t="s">
+        <v>164</v>
+      </c>
+      <c r="B95" t="s">
+        <v>189</v>
+      </c>
+      <c r="C95" t="s">
+        <v>165</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95" t="s">
+        <v>166</v>
+      </c>
+      <c r="F95" t="s">
+        <v>168</v>
+      </c>
+      <c r="G95" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96" t="s">
+        <v>164</v>
+      </c>
+      <c r="B96" t="s">
+        <v>188</v>
+      </c>
+      <c r="C96" t="s">
+        <v>165</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96" t="s">
+        <v>166</v>
+      </c>
+      <c r="F96" t="s">
+        <v>168</v>
+      </c>
+      <c r="G96" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" t="s">
+        <v>164</v>
+      </c>
+      <c r="B97" t="s">
+        <v>187</v>
+      </c>
+      <c r="C97" t="s">
+        <v>165</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97" t="s">
+        <v>166</v>
+      </c>
+      <c r="F97" t="s">
+        <v>168</v>
+      </c>
+      <c r="G97" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98" t="s">
+        <v>164</v>
+      </c>
+      <c r="B98" t="s">
+        <v>186</v>
+      </c>
+      <c r="C98" t="s">
+        <v>165</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98" t="s">
+        <v>166</v>
+      </c>
+      <c r="F98" t="s">
+        <v>168</v>
+      </c>
+      <c r="G98" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" t="s">
+        <v>164</v>
+      </c>
+      <c r="B99" t="s">
+        <v>185</v>
+      </c>
+      <c r="C99" t="s">
+        <v>165</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99" t="s">
+        <v>166</v>
+      </c>
+      <c r="F99" t="s">
+        <v>168</v>
+      </c>
+      <c r="G99" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100" t="s">
+        <v>164</v>
+      </c>
+      <c r="B100" t="s">
+        <v>184</v>
+      </c>
+      <c r="C100" t="s">
+        <v>165</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100" t="s">
+        <v>166</v>
+      </c>
+      <c r="F100" t="s">
+        <v>168</v>
+      </c>
+      <c r="G100" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
+      <c r="A101" t="s">
+        <v>164</v>
+      </c>
+      <c r="B101" t="s">
+        <v>183</v>
+      </c>
+      <c r="C101" t="s">
+        <v>165</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101" t="s">
+        <v>166</v>
+      </c>
+      <c r="F101" t="s">
+        <v>168</v>
+      </c>
+      <c r="G101" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" t="s">
+        <v>164</v>
+      </c>
+      <c r="B102" t="s">
+        <v>182</v>
+      </c>
+      <c r="C102" t="s">
+        <v>165</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+      <c r="E102" t="s">
+        <v>166</v>
+      </c>
+      <c r="F102" t="s">
+        <v>168</v>
+      </c>
+      <c r="G102" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" t="s">
+        <v>164</v>
+      </c>
+      <c r="B103" t="s">
+        <v>181</v>
+      </c>
+      <c r="C103" t="s">
+        <v>165</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103" t="s">
+        <v>166</v>
+      </c>
+      <c r="F103" t="s">
+        <v>168</v>
+      </c>
+      <c r="G103" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104" t="s">
+        <v>164</v>
+      </c>
+      <c r="B104" t="s">
+        <v>180</v>
+      </c>
+      <c r="C104" t="s">
+        <v>165</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+      <c r="E104" t="s">
+        <v>166</v>
+      </c>
+      <c r="F104" t="s">
+        <v>168</v>
+      </c>
+      <c r="G104" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105" t="s">
+        <v>164</v>
+      </c>
+      <c r="B105" t="s">
+        <v>179</v>
+      </c>
+      <c r="C105" t="s">
+        <v>165</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105" t="s">
+        <v>166</v>
+      </c>
+      <c r="F105" t="s">
+        <v>168</v>
+      </c>
+      <c r="G105" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
+      <c r="A106" t="s">
+        <v>164</v>
+      </c>
+      <c r="B106" t="s">
+        <v>178</v>
+      </c>
+      <c r="C106" t="s">
+        <v>165</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+      <c r="E106" t="s">
+        <v>166</v>
+      </c>
+      <c r="F106" t="s">
+        <v>168</v>
+      </c>
+      <c r="G106" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
+      <c r="A107" t="s">
+        <v>164</v>
+      </c>
+      <c r="B107" t="s">
+        <v>177</v>
+      </c>
+      <c r="C107" t="s">
+        <v>165</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107" t="s">
+        <v>166</v>
+      </c>
+      <c r="F107" t="s">
+        <v>168</v>
+      </c>
+      <c r="G107" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108" t="s">
+        <v>164</v>
+      </c>
+      <c r="B108" t="s">
+        <v>176</v>
+      </c>
+      <c r="C108" t="s">
+        <v>165</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+      <c r="E108" t="s">
+        <v>166</v>
+      </c>
+      <c r="F108" t="s">
+        <v>168</v>
+      </c>
+      <c r="G108" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
+      <c r="A109" t="s">
+        <v>164</v>
+      </c>
+      <c r="B109" t="s">
+        <v>175</v>
+      </c>
+      <c r="C109" t="s">
+        <v>165</v>
+      </c>
+      <c r="D109">
+        <v>0</v>
+      </c>
+      <c r="E109" t="s">
+        <v>166</v>
+      </c>
+      <c r="F109" t="s">
+        <v>168</v>
+      </c>
+      <c r="G109" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" t="s">
+        <v>164</v>
+      </c>
+      <c r="B110" t="s">
+        <v>174</v>
+      </c>
+      <c r="C110" t="s">
+        <v>165</v>
+      </c>
+      <c r="D110">
+        <v>0</v>
+      </c>
+      <c r="E110" t="s">
+        <v>166</v>
+      </c>
+      <c r="F110" t="s">
+        <v>168</v>
+      </c>
+      <c r="G110" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" t="s">
+        <v>164</v>
+      </c>
+      <c r="B111" t="s">
+        <v>173</v>
+      </c>
+      <c r="C111" t="s">
+        <v>165</v>
+      </c>
+      <c r="D111">
+        <v>0</v>
+      </c>
+      <c r="E111" t="s">
+        <v>166</v>
+      </c>
+      <c r="F111" t="s">
+        <v>168</v>
+      </c>
+      <c r="G111" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" t="s">
+        <v>164</v>
+      </c>
+      <c r="B112" t="s">
+        <v>172</v>
+      </c>
+      <c r="C112" t="s">
+        <v>165</v>
+      </c>
+      <c r="D112">
+        <v>0</v>
+      </c>
+      <c r="E112" t="s">
+        <v>166</v>
+      </c>
+      <c r="F112" t="s">
+        <v>168</v>
+      </c>
+      <c r="G112" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
+      <c r="A113" t="s">
+        <v>164</v>
+      </c>
+      <c r="B113" t="s">
+        <v>171</v>
+      </c>
+      <c r="C113" t="s">
+        <v>165</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+      <c r="E113" t="s">
+        <v>166</v>
+      </c>
+      <c r="F113" t="s">
+        <v>168</v>
+      </c>
+      <c r="G113" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
+      <c r="A114" t="s">
+        <v>164</v>
+      </c>
+      <c r="B114" t="s">
+        <v>170</v>
+      </c>
+      <c r="C114" t="s">
+        <v>165</v>
+      </c>
+      <c r="D114">
+        <v>0</v>
+      </c>
+      <c r="E114" t="s">
+        <v>166</v>
+      </c>
+      <c r="F114" t="s">
+        <v>168</v>
+      </c>
+      <c r="G114" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
+      <c r="A115" t="s">
+        <v>164</v>
+      </c>
+      <c r="B115" t="s">
+        <v>169</v>
+      </c>
+      <c r="C115" t="s">
+        <v>165</v>
+      </c>
+      <c r="D115">
+        <v>0</v>
+      </c>
+      <c r="E115" t="s">
+        <v>166</v>
+      </c>
+      <c r="F115" t="s">
+        <v>168</v>
+      </c>
+      <c r="G115" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="B1:B115">
+    <sortCondition descending="1" ref="B1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>